<commit_message>
Mise à jour des méta-données Apogée (février 2018)
</commit_message>
<xml_diff>
--- a/raw/Composante.xlsx
+++ b/raw/Composante.xlsx
@@ -1,11 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="270" yWindow="540" windowWidth="28215" windowHeight="12210"/>
+  </bookViews>
   <sheets>
     <sheet name="Composante" sheetId="1" r:id="rId1"/>
     <sheet name="Composante_commune" sheetId="2" r:id="rId2"/>
     <sheet name="Composante_type" sheetId="3" r:id="rId3"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -294,9 +300,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -304,13 +309,13 @@
     </font>
     <font>
       <sz val="9"/>
-      <color rgb="00333333"/>
+      <color rgb="FF333333"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
-      <color rgb="00FFFFFF"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -319,10 +324,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="00000000"/>
-        <bgColor rgb="00000000"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -353,31 +355,31 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="003877A6"/>
+        <color rgb="FF3877A6"/>
       </left>
       <right style="thin">
-        <color rgb="003877A6"/>
+        <color rgb="FF3877A6"/>
       </right>
       <top style="thin">
-        <color rgb="003877A6"/>
+        <color rgb="FF3877A6"/>
       </top>
       <bottom style="thin">
-        <color rgb="00A5A5B1"/>
+        <color rgb="FFA5A5B1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="00EBEBEB"/>
+        <color rgb="FFEBEBEB"/>
       </left>
       <right style="thin">
-        <color rgb="00EBEBEB"/>
+        <color rgb="FFEBEBEB"/>
       </right>
       <top style="thin">
-        <color rgb="00EBEBEB"/>
+        <color rgb="FFEBEBEB"/>
       </top>
       <bottom style="thin">
-        <color rgb="00EBEBEB"/>
+        <color rgb="FFEBEBEB"/>
       </bottom>
       <diagonal/>
     </border>
@@ -386,34 +388,333 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="bottom"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="bottom"/>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="bottom"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:E42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.1051986666667" customWidth="1"/>
-    <col min="2" max="5" width="10.7163133333333" customWidth="1"/>
-    <col min="6" max="6" width="4.67767866666667" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
+    <col min="2" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="26.1317" customHeight="1"/>
-    <row r="2" s="1" customFormat="1" ht="23.9985" customHeight="1">
+    <row r="1" spans="2:5" s="1" customFormat="1" ht="26.1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:5" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -427,7 +728,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="3" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
@@ -441,7 +742,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="4" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
@@ -455,7 +756,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="5" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
@@ -469,7 +770,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="6" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
@@ -483,7 +784,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="7" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>15</v>
       </c>
@@ -497,7 +798,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="8" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="s">
         <v>18</v>
       </c>
@@ -511,7 +812,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="9" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
         <v>21</v>
       </c>
@@ -525,7 +826,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="10" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="4" t="s">
         <v>23</v>
       </c>
@@ -539,7 +840,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="11" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
         <v>25</v>
       </c>
@@ -553,7 +854,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="12" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="4" t="s">
         <v>26</v>
       </c>
@@ -565,7 +866,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="13" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="3" t="s">
         <v>27</v>
       </c>
@@ -579,7 +880,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="14" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="4" t="s">
         <v>30</v>
       </c>
@@ -593,7 +894,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="15" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
         <v>32</v>
       </c>
@@ -607,7 +908,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="16" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="4" t="s">
         <v>34</v>
       </c>
@@ -621,7 +922,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="17" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="3" t="s">
         <v>36</v>
       </c>
@@ -635,7 +936,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="18" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="4" t="s">
         <v>38</v>
       </c>
@@ -649,7 +950,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="19" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="3" t="s">
         <v>40</v>
       </c>
@@ -663,7 +964,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="20" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="4" t="s">
         <v>42</v>
       </c>
@@ -677,7 +978,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="21" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="3" t="s">
         <v>44</v>
       </c>
@@ -691,7 +992,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="22" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="4" t="s">
         <v>46</v>
       </c>
@@ -705,7 +1006,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="23" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="3" t="s">
         <v>49</v>
       </c>
@@ -719,7 +1020,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="24" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="4" t="s">
         <v>51</v>
       </c>
@@ -733,7 +1034,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="25" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="3" t="s">
         <v>53</v>
       </c>
@@ -747,7 +1048,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="26" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="4" t="s">
         <v>55</v>
       </c>
@@ -761,7 +1062,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="27" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="3" t="s">
         <v>57</v>
       </c>
@@ -775,7 +1076,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="28" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="4" t="s">
         <v>59</v>
       </c>
@@ -789,7 +1090,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="29" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="3" t="s">
         <v>29</v>
       </c>
@@ -803,7 +1104,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="30" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="4" t="s">
         <v>61</v>
       </c>
@@ -817,7 +1118,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="31" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="3" t="s">
         <v>63</v>
       </c>
@@ -831,7 +1132,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="32" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="4" t="s">
         <v>65</v>
       </c>
@@ -845,7 +1146,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="33" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="3" t="s">
         <v>66</v>
       </c>
@@ -859,7 +1160,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="34" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="4" t="s">
         <v>67</v>
       </c>
@@ -873,7 +1174,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="35" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="3" t="s">
         <v>69</v>
       </c>
@@ -887,7 +1188,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="36" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="4" t="s">
         <v>71</v>
       </c>
@@ -901,7 +1202,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="37" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="37" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="3" t="s">
         <v>73</v>
       </c>
@@ -915,7 +1216,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="38" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="4" t="s">
         <v>76</v>
       </c>
@@ -929,7 +1230,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="39" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="39" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="3" t="s">
         <v>78</v>
       </c>
@@ -943,7 +1244,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="40" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="4" t="s">
         <v>80</v>
       </c>
@@ -957,7 +1258,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="41" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="3" t="s">
         <v>81</v>
       </c>
@@ -971,24 +1272,29 @@
         <v>61</v>
       </c>
     </row>
-    <row r="42" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
+    <row r="42" spans="2:5" s="1" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <pageSetup paperSize="9" scale="100" orientation="portrait"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.8129" customWidth="1"/>
-    <col min="2" max="3" width="10.7163133333333" customWidth="1"/>
-    <col min="4" max="4" width="4.67767866666667" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" customWidth="1"/>
+    <col min="2" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="5.333" customHeight="1"/>
-    <row r="2" s="1" customFormat="1" ht="23.9985" customHeight="1">
+    <row r="1" spans="2:3" s="1" customFormat="1" ht="5.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:3" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
@@ -996,7 +1302,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="3" spans="2:3" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>75</v>
       </c>
@@ -1004,7 +1310,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="4" spans="2:3" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>13</v>
       </c>
@@ -1012,7 +1318,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="5" spans="2:3" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>17</v>
       </c>
@@ -1020,7 +1326,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="6" spans="2:3" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>48</v>
       </c>
@@ -1028,7 +1334,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="7" spans="2:3" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1036,7 +1342,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="8" spans="2:3" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="s">
         <v>20</v>
       </c>
@@ -1044,29 +1350,34 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" s="1" customFormat="1" ht="11.1993" customHeight="1">
+    <row r="9" spans="2:3" s="1" customFormat="1" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
+    <row r="10" spans="2:3" s="1" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <pageSetup paperSize="9" scale="100" orientation="portrait"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.8165" customWidth="1"/>
-    <col min="2" max="2" width="10.7163133333333" customWidth="1"/>
-    <col min="3" max="3" width="42.6397" customWidth="1"/>
-    <col min="4" max="4" width="4.67767866666667" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="42.5703125" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="5.333" customHeight="1"/>
-    <row r="2" s="1" customFormat="1" ht="23.9985" customHeight="1">
+    <row r="1" spans="2:3" s="1" customFormat="1" ht="5.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:3" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1074,7 +1385,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="3" spans="2:3" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
@@ -1082,7 +1393,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="4" spans="2:3" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>29</v>
       </c>
@@ -1090,7 +1401,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="5" spans="2:3" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>61</v>
       </c>
@@ -1098,7 +1409,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="6" spans="2:3" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
@@ -1106,7 +1417,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" ht="19.7321" customHeight="1">
+    <row r="7" spans="2:3" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>14</v>
       </c>
@@ -1114,9 +1425,10 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
+    <row r="8" spans="2:3" s="1" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <pageSetup paperSize="9" scale="100" orientation="portrait"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Mise à jour apogée d'avril 2018
</commit_message>
<xml_diff>
--- a/raw/Composante.xlsx
+++ b/raw/Composante.xlsx
@@ -1,17 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <bookViews>
-    <workbookView xWindow="270" yWindow="540" windowWidth="28215" windowHeight="12210"/>
-  </bookViews>
   <sheets>
     <sheet name="Composante" sheetId="1" r:id="rId1"/>
     <sheet name="Composante_commune" sheetId="2" r:id="rId2"/>
     <sheet name="Composante_type" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -300,8 +294,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -309,13 +304,13 @@
     </font>
     <font>
       <sz val="9"/>
-      <color rgb="FF333333"/>
+      <color rgb="00333333"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="00FFFFFF"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -324,7 +319,10 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="gray125">
+        <fgColor rgb="00000000"/>
+        <bgColor rgb="00000000"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -355,31 +353,31 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3877A6"/>
+        <color rgb="003877A6"/>
       </left>
       <right style="thin">
-        <color rgb="FF3877A6"/>
+        <color rgb="003877A6"/>
       </right>
       <top style="thin">
-        <color rgb="FF3877A6"/>
+        <color rgb="003877A6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFA5A5B1"/>
+        <color rgb="00A5A5B1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFEBEBEB"/>
+        <color rgb="00EBEBEB"/>
       </left>
       <right style="thin">
-        <color rgb="FFEBEBEB"/>
+        <color rgb="00EBEBEB"/>
       </right>
       <top style="thin">
-        <color rgb="FFEBEBEB"/>
+        <color rgb="00EBEBEB"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFEBEBEB"/>
+        <color rgb="00EBEBEB"/>
       </bottom>
       <diagonal/>
     </border>
@@ -388,333 +386,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="1F497D"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="EEECE1"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4F81BD"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="C0504D"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9BBB59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064A2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4BACC6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="F79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000FF"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="800080"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView rightToLeft="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.140625" customWidth="1"/>
-    <col min="2" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="1" max="1" width="21.1051986666667" customWidth="1"/>
+    <col min="2" max="5" width="10.7163133333333" customWidth="1"/>
+    <col min="6" max="6" width="4.67767866666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" s="1" customFormat="1" ht="26.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:5" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" s="1" customFormat="1" ht="26.1317" customHeight="1"/>
+    <row r="2" s="1" customFormat="1" ht="23.9985" customHeight="1">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -728,7 +430,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
@@ -742,7 +444,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
@@ -756,7 +458,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
@@ -770,7 +472,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
@@ -784,7 +486,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B7" s="3" t="s">
         <v>15</v>
       </c>
@@ -798,7 +500,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B8" s="4" t="s">
         <v>18</v>
       </c>
@@ -812,7 +514,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B9" s="3" t="s">
         <v>21</v>
       </c>
@@ -826,7 +528,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B10" s="4" t="s">
         <v>23</v>
       </c>
@@ -840,7 +542,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B11" s="3" t="s">
         <v>25</v>
       </c>
@@ -854,7 +556,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B12" s="4" t="s">
         <v>26</v>
       </c>
@@ -866,7 +568,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B13" s="3" t="s">
         <v>27</v>
       </c>
@@ -880,7 +582,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B14" s="4" t="s">
         <v>30</v>
       </c>
@@ -894,7 +596,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B15" s="3" t="s">
         <v>32</v>
       </c>
@@ -908,7 +610,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B16" s="4" t="s">
         <v>34</v>
       </c>
@@ -922,7 +624,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B17" s="3" t="s">
         <v>36</v>
       </c>
@@ -936,7 +638,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B18" s="4" t="s">
         <v>38</v>
       </c>
@@ -950,7 +652,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B19" s="3" t="s">
         <v>40</v>
       </c>
@@ -964,7 +666,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B20" s="4" t="s">
         <v>42</v>
       </c>
@@ -978,7 +680,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B21" s="3" t="s">
         <v>44</v>
       </c>
@@ -992,7 +694,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B22" s="4" t="s">
         <v>46</v>
       </c>
@@ -1006,7 +708,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B23" s="3" t="s">
         <v>49</v>
       </c>
@@ -1020,7 +722,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B24" s="4" t="s">
         <v>51</v>
       </c>
@@ -1034,7 +736,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B25" s="3" t="s">
         <v>53</v>
       </c>
@@ -1048,7 +750,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B26" s="4" t="s">
         <v>55</v>
       </c>
@@ -1062,7 +764,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B27" s="3" t="s">
         <v>57</v>
       </c>
@@ -1076,7 +778,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B28" s="4" t="s">
         <v>59</v>
       </c>
@@ -1090,7 +792,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B29" s="3" t="s">
         <v>29</v>
       </c>
@@ -1104,7 +806,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B30" s="4" t="s">
         <v>61</v>
       </c>
@@ -1118,7 +820,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B31" s="3" t="s">
         <v>63</v>
       </c>
@@ -1132,7 +834,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B32" s="4" t="s">
         <v>65</v>
       </c>
@@ -1146,7 +848,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B33" s="3" t="s">
         <v>66</v>
       </c>
@@ -1160,7 +862,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B34" s="4" t="s">
         <v>67</v>
       </c>
@@ -1174,7 +876,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B35" s="3" t="s">
         <v>69</v>
       </c>
@@ -1188,7 +890,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B36" s="4" t="s">
         <v>71</v>
       </c>
@@ -1202,7 +904,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="37" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B37" s="3" t="s">
         <v>73</v>
       </c>
@@ -1216,7 +918,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B38" s="4" t="s">
         <v>76</v>
       </c>
@@ -1230,7 +932,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B39" s="3" t="s">
         <v>78</v>
       </c>
@@ -1244,7 +946,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B40" s="4" t="s">
         <v>80</v>
       </c>
@@ -1258,7 +960,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="2:5" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B41" s="3" t="s">
         <v>81</v>
       </c>
@@ -1272,29 +974,27 @@
         <v>61</v>
       </c>
     </row>
-    <row r="42" spans="2:5" s="1" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" scale="100" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView rightToLeft="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" customWidth="1"/>
-    <col min="2" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="1" max="1" width="25.8129" customWidth="1"/>
+    <col min="2" max="3" width="10.7163133333333" customWidth="1"/>
+    <col min="4" max="4" width="4.67767866666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" s="1" customFormat="1" ht="5.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:3" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" s="1" customFormat="1" ht="5.333" customHeight="1"/>
+    <row r="2" s="1" customFormat="1" ht="23.9985" customHeight="1">
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1302,7 +1002,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="2:3" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B3" s="3" t="s">
         <v>75</v>
       </c>
@@ -1310,7 +1010,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="2:3" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B4" s="4" t="s">
         <v>13</v>
       </c>
@@ -1318,7 +1018,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="2:3" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B5" s="3" t="s">
         <v>17</v>
       </c>
@@ -1326,7 +1026,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="2:3" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B6" s="4" t="s">
         <v>48</v>
       </c>
@@ -1334,7 +1034,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="2:3" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1342,7 +1042,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="2:3" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B8" s="4" t="s">
         <v>20</v>
       </c>
@@ -1350,34 +1050,32 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="2:3" s="1" customFormat="1" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" s="1" customFormat="1" ht="11.1993" customHeight="1">
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="2:3" s="1" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" scale="100" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView rightToLeft="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="42.5703125" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.8165" customWidth="1"/>
+    <col min="2" max="2" width="10.7163133333333" customWidth="1"/>
+    <col min="3" max="3" width="42.6397" customWidth="1"/>
+    <col min="4" max="4" width="4.67767866666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" s="1" customFormat="1" ht="5.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:3" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" s="1" customFormat="1" ht="5.333" customHeight="1"/>
+    <row r="2" s="1" customFormat="1" ht="23.9985" customHeight="1">
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1385,7 +1083,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="2:3" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
@@ -1393,7 +1091,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="2:3" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B4" s="4" t="s">
         <v>29</v>
       </c>
@@ -1401,7 +1099,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="2:3" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B5" s="3" t="s">
         <v>61</v>
       </c>
@@ -1409,7 +1107,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="2:3" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
@@ -1417,7 +1115,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="2:3" s="1" customFormat="1" ht="19.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B7" s="3" t="s">
         <v>14</v>
       </c>
@@ -1425,10 +1123,9 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="2:3" s="1" customFormat="1" ht="28.7" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" scale="100" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>